<commit_message>
polished something detail about 计分表 and added a file about the Wechat official account requiremrnt
</commit_message>
<xml_diff>
--- a/Docs/计分组/2015-THU-计分表.xlsx
+++ b/Docs/计分组/2015-THU-计分表.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git work\2015-Tsinghua-XLP-CDT\Docs\计分组\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18500" windowHeight="13740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18495" windowHeight="13740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="day 1" sheetId="1" r:id="rId1"/>
     <sheet name="day2（有重分组）" sheetId="2" r:id="rId2"/>
     <sheet name="day3（有重分组）" sheetId="3" r:id="rId3"/>
-    <sheet name="工作表4" sheetId="4" r:id="rId4"/>
+    <sheet name="day4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -267,6 +272,10 @@
   </si>
   <si>
     <t>额外加分扣分</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>当天总分</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -377,16 +386,24 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -712,28 +729,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18.125" customWidth="1"/>
+    <col min="13" max="13" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,188 +790,191 @@
       <c r="M1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -973,26 +993,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
     <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1"/>
+    <col min="11" max="11" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,188 +1046,191 @@
       <c r="K1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -1226,23 +1249,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="A1:XFD1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,188 +1290,191 @@
       <c r="H1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -1467,23 +1493,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
     <col min="4" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1511,188 +1537,191 @@
       <c r="I1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>

</xml_diff>